<commit_message>
Add a little content in excel
</commit_message>
<xml_diff>
--- a/多介质模型文献阅读/Excel文献拆解/多介质模型文献整理-P1.xlsx
+++ b/多介质模型文献阅读/Excel文献拆解/多介质模型文献整理-P1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\10月Parabens文献调研\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python learning\GirKarken\ReadPaper in Excel\多介质模型文献阅读\Excel文献拆解\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="博士论文阅读" sheetId="3" r:id="rId1"/>
@@ -5190,8 +5190,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6312,7 +6312,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add analyses of papers of shijie
加入了对师姐文章的解读
</commit_message>
<xml_diff>
--- a/多介质模型文献阅读/Excel文献拆解/多介质模型文献整理-P1.xlsx
+++ b/多介质模型文献阅读/Excel文献拆解/多介质模型文献整理-P1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,36 +12,145 @@
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="博士论文阅读" sheetId="3" r:id="rId1"/>
-    <sheet name="英文综述阅读" sheetId="12" r:id="rId2"/>
-    <sheet name="中文综述阅读" sheetId="13" r:id="rId3"/>
-    <sheet name="英文期刊阅读" sheetId="4" r:id="rId4"/>
-    <sheet name="速读十问" sheetId="11" r:id="rId5"/>
-    <sheet name="物化性质文献 " sheetId="7" r:id="rId6"/>
-    <sheet name="Mackay" sheetId="9" r:id="rId7"/>
-    <sheet name="Film" sheetId="5" r:id="rId8"/>
-    <sheet name="Dust" sheetId="8" r:id="rId9"/>
-    <sheet name="基金" sheetId="10" r:id="rId10"/>
-    <sheet name="搜索技巧" sheetId="6" r:id="rId11"/>
+    <sheet name="组内论文" sheetId="14" r:id="rId1"/>
+    <sheet name="博士论文阅读" sheetId="3" r:id="rId2"/>
+    <sheet name="英文综述阅读" sheetId="12" r:id="rId3"/>
+    <sheet name="赵雪博士论文拆解1" sheetId="15" r:id="rId4"/>
+    <sheet name="中文综述阅读" sheetId="13" r:id="rId5"/>
+    <sheet name="英文期刊阅读" sheetId="4" r:id="rId6"/>
+    <sheet name="速读十问" sheetId="11" r:id="rId7"/>
+    <sheet name="物化性质文献 " sheetId="7" r:id="rId8"/>
+    <sheet name="Mackay" sheetId="9" r:id="rId9"/>
+    <sheet name="Film" sheetId="5" r:id="rId10"/>
+    <sheet name="Dust" sheetId="8" r:id="rId11"/>
+    <sheet name="基金" sheetId="10" r:id="rId12"/>
+    <sheet name="搜索技巧" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="O2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本文档将“研究对象”视为污染物，
+而“数据收集对象”视为利用科学手段所认识的对象，即环境介质、人体生物样品、产品等。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+数据收集工具即认识对象的工具，即我们定量表征事物属性的工具或者方法</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+利用数据收集工具对数据收集对象进行的一系列的操作，从而得到数据区的数据内容。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+对表格的数据进行处理的方法和步骤</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Administrator</author>
@@ -77,7 +186,72 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>User</author>
+  </authors>
+  <commentList>
+    <comment ref="I4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+城市污水是parabens及其代谢物在城市河流中的重要污染点源。
+城市污水→城市排水系统（排水管道和污水处理厂）→受纳水体</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+城市地表径流是大气颗粒物、地面积尘、土壤和垃圾渗滤液等环境介质中的污染物进入城市水环境的重要途径，是重要的面源污染。
+地面积尘、土壤→地表径流→受纳水体
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>User</author>
@@ -443,7 +617,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>User</author>
@@ -559,7 +733,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="341">
   <si>
     <t>年份</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4002,6 +4176,679 @@
   </si>
   <si>
     <t>科学通报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZXSJ01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improving urban drainage systems to mitigate 
+PPCPs in surface water: a watershed perspective</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZXSJ02</t>
+  </si>
+  <si>
+    <t>ZXSJ03</t>
+  </si>
+  <si>
+    <t>ZXSJ04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Road runoff as a significant nonpoint source of 
+parabens and their metabolites in urban rivers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ecotoxicology and 
+Environmental Safety</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Journal of Hazardous 
+Materials</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>主要结果</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>结论</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Xue Zhao
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>赵雪</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wenhui Qiu
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">裘文慧
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Yi Zheng
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>郑一</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Occurrence, distribution, bioaccumulation, and ecological risk of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bisphenol analogues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, parabens and their metabolites in the Pearl River Estuary</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yi Zheng
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>郑一</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中国环境科学</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>雄安新区水环境中对羟基苯甲酸酯含量及风险</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.Abstract: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">This study analyzed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">eight bisphenol analogues, six parabens, and five paraben metabolites </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in seawater (including aqueous and suspended particle matter (SPM)), as well as organism samples from the Pearl River Estuary, in order to determine their occurrence, distribution, bioaccumulation, and ecological and human health risk in South China's marine environment.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pearl River Estuary </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Seawater sample (aqueous samples + SPM), S1-S25, 2017-12
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Samples of marine organisms (shellfish species11, fish species10), 2017-12</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对象</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>检测方法：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Wanli Ma, 2018, Concentrations and fate of parabens and their metabolites in two typical wastewater treatment plants in northeastern China
+SPM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和对象二检测方法：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Xue, X., Kannan, K., 2017, Trophic magnification of parabens and their metabolites in a Subtropical marine food web</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>论文编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈尔滨工业大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>环境科学与工程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赵雪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市化流域水环境中对羟基苯甲酸酯的源汇过程研究</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parabens</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深圳市茅洲河流域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>河水111、河流表层沉积物65、污水处理厂进水20、
+污水处理厂出水29、地面积尘21、土壤12、路面地表径流37、雨水管径流3、海水样品37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BS004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摘要</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背景
+研究空白
+研究主题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>城市化河流中对轻基苯甲酸酯及其代谢物的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>污染特征</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>及其</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>受城市建设和管理措施影响的机制</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要研究内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要研究内容1的主要结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同环境介质中的浓度水平结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…平均浓度…对比发现…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>河水中目标污染物的来源
+主要结论/发现：排水体制改造前，</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合流制溢流排水</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是导致茅洲河河水中对羟基苯甲酸酯及其代谢物异常增高的主要原因。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过分流制排水体制改造，目标污染物进入河段的总量可减少80%以上。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要研究内容2的主要结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段六</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要研究内容3的主要结果</t>
+  </si>
+  <si>
+    <t>段七</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究意义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>答辩PPT的第9页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂的城市排水系统如何影响城市水环境中Parabens及其代谢物的污染？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>答辩PPT的第10页</t>
+  </si>
+  <si>
+    <t>在降雨径流的驱动下，
+面源污染过程如何影响城市水环境中Parabens及其代谢物的污染？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>通过固相萃取和液液萃取结合
+液相色谱质谱联用仪分析测定了不同介质中对羟基苯甲酸酯及其代谢物的浓度水平。
+1.分析了典型城市雨源型河流中对轻基苯甲酸酯及其代谢物的污染特征及来源构成；
+（解析城市化流域水环境中parabens及其代谢物污染的时空特征及其影响因素）
+2.研究了城市河流中目标污染物的点源污染过程及其影响机制；
+（揭示城市复杂排水系统对雨源型河流中parabens及其代谢物</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>点源污染过程</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的影响机制）
+3.量化了城市</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>面源污染过程</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>对城市河流中目标污染物的贡献
+（阐明城市路面地表径流对于城市水环境中parabens及其代谢物污染的贡献）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应文章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应章节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三章：城市雨源型河流的污染</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四章：城市化流域的点源污染过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第五章：城市化流域的面源污
+染过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初期冲刷效应、
+面源污染影响的定量分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Occurrence, distribution, bioaccumulation, and ecological risk of bisphenol analogues, parabens and their metabolites in the Pearl River Estuary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4009,7 +4856,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4145,6 +4992,28 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="11">
@@ -4295,7 +5164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4423,6 +5292,45 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4468,16 +5376,305 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 17" descr="https://pubs.acs.org/cms/10.1021/es2003233/asset/images/large/es-2011-003233_0005.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2334169F-9FD6-4EE8-BEEE-F273036F1D93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8282940" y="9715500"/>
+          <a:ext cx="304800" cy="289560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197226</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>233084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3720354</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1664355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE7F118-C7A7-53C1-2EA4-8211812F2DBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9646026" y="842684"/>
+          <a:ext cx="3523128" cy="1431271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>111474</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>232303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3837957</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1730189</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AC062C6-F1E8-346E-75D0-BEA6BB08D48F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9560274" y="2751385"/>
+          <a:ext cx="3726483" cy="1497886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>94770</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>99252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3810594</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2166258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E504BDA8-E44D-AADD-57CC-F7A80622164E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9521799" y="6423852"/>
+          <a:ext cx="3715824" cy="2067006"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>866776</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3038476</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1895780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11630026" y="2257425"/>
+          <a:ext cx="2171700" cy="1886255"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>305</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3751336</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2505075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972800" y="4219575"/>
+          <a:ext cx="3541786" cy="2438400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>771525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3287949</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3200400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4494,8 +5691,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11458576" y="2266950"/>
-          <a:ext cx="2171700" cy="1886255"/>
+          <a:off x="6267450" y="2105025"/>
+          <a:ext cx="3249849" cy="2428875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4507,7 +5704,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4524,7 +5721,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2" descr="https://d3i71xaburhd42.cloudfront.net/74bbf259c13521e68161501e0de5668e36354a71/4-Figure1-1.png"/>
+        <xdr:cNvPr id="3" name="图片 2" descr="https://d3i71xaburhd42.cloudfront.net/74bbf259c13521e68161501e0de5668e36354a71/4-Figure1-1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4573,13 +5776,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>2914650</xdr:colOff>
+      <xdr:colOff>2815590</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>1861134</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4617,7 +5826,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4649,13 +5864,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>4476750</xdr:colOff>
+      <xdr:colOff>4210050</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>2485876</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="图片 6"/>
+        <xdr:cNvPr id="7" name="图片 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4693,7 +5914,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2065" name="AutoShape 17" descr="https://pubs.acs.org/cms/10.1021/es2003233/asset/images/large/es-2011-003233_0005.jpeg"/>
+        <xdr:cNvPr id="2065" name="AutoShape 17" descr="https://pubs.acs.org/cms/10.1021/es2003233/asset/images/large/es-2011-003233_0005.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4735,7 +5962,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="图片 7"/>
+        <xdr:cNvPr id="8" name="图片 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4779,7 +6012,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4805,7 +6044,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4822,7 +6061,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4860,7 +6105,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4898,7 +6149,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5187,341 +6444,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="1"/>
-    <col min="4" max="4" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="1"/>
-    <col min="7" max="7" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="52.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="38.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="46.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="46.75" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="64.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="47.875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="63.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57" style="1" customWidth="1"/>
+    <col min="9" max="9" width="90.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="45.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="40.375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="49.625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="46.75" style="1" customWidth="1"/>
+    <col min="19" max="19" width="61.375" style="1" customWidth="1"/>
     <col min="20" max="20" width="76.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+    </row>
+    <row r="2" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="M2" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="S2" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="16">
         <v>2019</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="81" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="D3" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+    </row>
+    <row r="4" spans="1:23" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="2">
-        <v>2016</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="C4" s="16">
+        <v>2021</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+    </row>
+    <row r="5" spans="1:23" s="46" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="16">
+        <v>2021</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" ht="179.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="16">
         <v>2022</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D6" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+    </row>
+    <row r="7" spans="1:23" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
-      <c r="B7" s="24"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -5540,10 +6743,11 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="24"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -5562,52 +6766,32 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:R1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5617,6 +6801,320 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="146.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1998</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="61.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="16">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2001</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="146.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
@@ -5886,7 +7384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E6"/>
@@ -5963,6 +7461,457 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:T10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="1"/>
+    <col min="4" max="4" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="1"/>
+    <col min="7" max="7" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="38.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="46.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="46.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="64.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="63.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="76.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="81" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2022</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" ht="200.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="2">
+        <v>2022</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -5970,7 +7919,7 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="32"/>
     <col min="2" max="2" width="9.5" style="32" bestFit="1" customWidth="1"/>
@@ -6127,7 +8076,232 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="5" width="27.375" style="49" customWidth="1"/>
+    <col min="6" max="6" width="43.5" style="49" customWidth="1"/>
+    <col min="7" max="7" width="31.375" style="49" customWidth="1"/>
+    <col min="8" max="8" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.625" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="55" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="I2" s="56"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50" t="s">
+        <v>310</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="297" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52" t="s">
+        <v>313</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52" t="s">
+        <v>316</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>340</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>336</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>315</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>321</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>337</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>322</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>339</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" s="50" t="s">
+        <v>338</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>324</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -6135,7 +8309,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
@@ -6307,13 +8481,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6358,28 +8532,28 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="45" t="s">
+      <c r="J1" s="61"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="44" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
       <c r="AB1" s="16"/>
       <c r="AC1" s="16"/>
     </row>
@@ -6992,7 +9166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -7000,7 +9174,7 @@
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
     <col min="8" max="9" width="26.125" style="1" bestFit="1" customWidth="1"/>
@@ -7016,27 +9190,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="64" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="52" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
     </row>
     <row r="2" spans="1:17" ht="27" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
@@ -7101,7 +9275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -7240,7 +9414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
@@ -7288,27 +9462,27 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="45" t="s">
+      <c r="J1" s="61"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="44" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
       <c r="AA1" s="16"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -7631,318 +9805,4 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="146.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.875" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="16">
-        <v>1998</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="61.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="16">
-        <v>2000</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="16">
-        <v>2001</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="146.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.875" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>